<commit_message>
newest changes to trigram model
</commit_message>
<xml_diff>
--- a/neural-network/trigram-pattern-frequencies/trigram-pattern-frequencies-test.xlsx
+++ b/neural-network/trigram-pattern-frequencies/trigram-pattern-frequencies-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a66692c83fa18ac/Desktop/relationships-between-organizational-patterns/neural-network/trigram-pattern-frequencies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a66692c83fa18ac/Desktop/temp/relationships-between-organizational-patterns/neural-network/trigram-pattern-frequencies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{EFC78230-4D74-4026-9CA1-27BEDAABD1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0811A6D6-1BAF-47F4-B88D-37966C712627}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ED33FE0F-5BD9-48CF-B61F-F95F8F682754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{731B3B62-FE4A-424E-9540-29D236651053}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{728EA022-8D32-49BB-B38B-E0E06FC25055}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>OrganizationalPattern</t>
   </si>
@@ -95,6 +95,39 @@
   </si>
   <si>
     <t>VariationBehindInterface</t>
+  </si>
+  <si>
+    <t>DomainExpertiseInRoles</t>
+  </si>
+  <si>
+    <t>FeatureAssignment</t>
+  </si>
+  <si>
+    <t>FewRoles</t>
+  </si>
+  <si>
+    <t>GenericsAndSpecifics</t>
+  </si>
+  <si>
+    <t>HierarchyOfFactories</t>
+  </si>
+  <si>
+    <t>LockEmUpTogether</t>
+  </si>
+  <si>
+    <t>LooseInterfaces</t>
+  </si>
+  <si>
+    <t>OrganizationFollowsMarket</t>
+  </si>
+  <si>
+    <t>ArchitectureTeam</t>
+  </si>
+  <si>
+    <t>CodeOwnership</t>
+  </si>
+  <si>
+    <t>DistributeWorkEvenly</t>
   </si>
 </sst>
 </file>
@@ -483,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFD514A-2A61-4381-8EA3-92A13EBF2E60}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,6 +866,457 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M18" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M19" s="3">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>